<commit_message>
changed feedback ui and added student tab
</commit_message>
<xml_diff>
--- a/public/sample_faculty.xlsx
+++ b/public/sample_faculty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\Feedback System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454F3A27-C2A3-4D6C-B160-78E3AD23355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBF6CD-86FB-43C0-9B3E-6C0788AA371C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6036" yWindow="3936" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,46 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>discipline_name</t>
-  </si>
-  <si>
-    <t>branch_name</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
-    <t>Advanced Data Structures</t>
-  </si>
-  <si>
-    <t>Engineering Management</t>
-  </si>
-  <si>
-    <t>Network System and Securities</t>
-  </si>
-  <si>
-    <t>Digital Image Processing</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>faculty_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>discipline_id</t>
+  </si>
+  <si>
+    <t>branch_id</t>
+  </si>
+  <si>
+    <t>exceel@gmail.com</t>
+  </si>
+  <si>
+    <t>ME specialist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,13 +86,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,21 +377,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -395,63 +401,46 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>7418529633</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E2">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1EFF113B-EA9B-47AC-A8BF-D97DEDC77399}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>